<commit_message>
kgc pipeline simplified, paths modified in config and mappings
</commit_message>
<xml_diff>
--- a/mappings/solarchem-mapping.xlsx
+++ b/mappings/solarchem-mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/knowledge-graph/mappings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-kg/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEC3420-F934-CE47-B86A-D4BB8DA2D8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C657B674-50B7-5145-A270-903FCB1BF420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28740" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="28740" windowHeight="17500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Predicate_Object" sheetId="4" r:id="rId4"/>
     <sheet name="Function" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Source!$A$1:$C$56</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -154,9 +157,6 @@
     <t>format</t>
   </si>
   <si>
-    <t>data/catalystsdata.csv</t>
-  </si>
-  <si>
     <t>csv</t>
   </si>
   <si>
@@ -592,9 +592,6 @@
     <t>schema:ScholarlyArticle</t>
   </si>
   <si>
-    <t>data/papersOA.json</t>
-  </si>
-  <si>
     <t>JSONPath</t>
   </si>
   <si>
@@ -613,9 +610,6 @@
     <t>{uri}</t>
   </si>
   <si>
-    <t>data/chemicals.csv</t>
-  </si>
-  <si>
     <t>CO-CATALYST4</t>
   </si>
   <si>
@@ -746,6 +740,15 @@
   </si>
   <si>
     <t>https://w3id.org/solar/i/Article/{No_de_Ref}</t>
+  </si>
+  <si>
+    <t>../mappings/data/papersOA.json</t>
+  </si>
+  <si>
+    <t>../mappings/data/catalystsdata.csv</t>
+  </si>
+  <si>
+    <t>../mappings/data/chemicals.csv</t>
   </si>
 </sst>
 </file>
@@ -864,9 +867,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -904,7 +907,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1010,7 +1013,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1152,7 +1155,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1171,7 +1174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1243,7 +1246,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1251,7 +1254,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1259,55 +1262,55 @@
         <v>28</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1315,7 +1318,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1351,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1382,7 +1385,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1393,7 +1396,7 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1401,582 +1404,582 @@
         <v>29</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>185</v>
+        <v>229</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2018,282 +2021,282 @@
         <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
         <v>42</v>
       </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
       <c r="C6" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" t="s">
         <v>140</v>
       </c>
-      <c r="B24" t="s">
-        <v>141</v>
-      </c>
       <c r="C24" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>180</v>
+      </c>
+      <c r="C27" t="s">
         <v>182</v>
-      </c>
-      <c r="C27" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2366,7 +2369,7 @@
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>14</v>
@@ -2383,10 +2386,10 @@
         <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="1"/>
@@ -2399,10 +2402,10 @@
         <v>29</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="1"/>
@@ -2415,10 +2418,10 @@
         <v>29</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>156</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="1"/>
@@ -2431,10 +2434,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="1"/>
@@ -2447,13 +2450,13 @@
         <v>29</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2465,10 +2468,10 @@
         <v>29</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>162</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="1"/>
@@ -2481,10 +2484,10 @@
         <v>29</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="1"/>
@@ -2497,10 +2500,10 @@
         <v>29</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>166</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="1"/>
@@ -2513,13 +2516,13 @@
         <v>29</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2531,31 +2534,31 @@
         <v>29</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>169</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>170</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="1"/>
@@ -2565,16 +2568,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2583,13 +2586,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>172</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>173</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="1"/>
@@ -2599,27 +2602,27 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -2627,16 +2630,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>45</v>
-      </c>
       <c r="D17" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -2644,16 +2647,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="D18" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -2661,16 +2664,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -2678,13 +2681,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -2693,16 +2696,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -2710,16 +2713,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -2727,36 +2730,36 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -2764,16 +2767,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -2781,16 +2784,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -2798,16 +2801,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -2815,13 +2818,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -2830,16 +2833,16 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -2847,376 +2850,376 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="C30" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H35" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H43" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="D44" s="7"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H47" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B49" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="D49" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H51" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>135</v>
       </c>
       <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B54" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>138</v>
-      </c>
       <c r="D54" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="7"/>
@@ -3224,635 +3227,635 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H55" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C79" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B79" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>145</v>
-      </c>
       <c r="D79" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>